<commit_message>
Work from thursday. I have distribution and override working on odk side. BUT I tried to set up a callback that will query to see if a distribution already exists and then have a callback function that if failed it will create the override. And that doesn't work. However, the code is still in there, just commented out (authorizations_detail.js)
</commit_message>
<xml_diff>
--- a/app/config/tables/deployment/forms/deploy_to_specific/deploy_to_specific.xlsx
+++ b/app/config/tables/deployment/forms/deploy_to_specific/deploy_to_specific.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="99">
   <si>
     <t>type</t>
   </si>
@@ -143,181 +143,184 @@
     <t>No</t>
   </si>
   <si>
+    <t>min_range</t>
+  </si>
+  <si>
+    <t>max_range</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>pre-deployment</t>
+  </si>
+  <si>
+    <t>We will now distribute the appropriate item pack</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>Scan an item pack barcode within the range of {{data.min_range}} to {{data.max_range}}</t>
+  </si>
+  <si>
+    <t>item_scan</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>(data('scanned_item_pack_barcode') &gt; data('maxRange')) || (data('scanned_item_pack_barcode') &lt; data('minRange'))</t>
+  </si>
+  <si>
+    <t>select_one</t>
+  </si>
+  <si>
+    <t>try_again</t>
+  </si>
+  <si>
+    <t>Unauthorized Item Pack! Do not distribute this  item pack. Would you like to scan a different item pack?</t>
+  </si>
+  <si>
+    <t>selected(data('try_again'),'yes')</t>
+  </si>
+  <si>
+    <t>goto item_scan</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>This item pack is authorized. Please distribute this item pack.</t>
+  </si>
+  <si>
+    <t>linked_table</t>
+  </si>
+  <si>
+    <t>Please click the pencil icon to record distribution</t>
+  </si>
+  <si>
+    <t>begin screen</t>
+  </si>
+  <si>
+    <t>Please continue to the next screen if you have clicked the pencil icon to record distribution</t>
+  </si>
+  <si>
+    <t>async_assign_single_string</t>
+  </si>
+  <si>
+    <t>is_distributed_value_query</t>
+  </si>
+  <si>
+    <t>end screen</t>
+  </si>
+  <si>
+    <t>data('is_distributed') == 'true'</t>
+  </si>
+  <si>
+    <t>pre-summary</t>
+  </si>
+  <si>
+    <t>Since the authorized item pack was successfully distributed, we will complete now complete a brief report.</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>now()</t>
+  </si>
+  <si>
+    <t>What is the name of the distributor?</t>
+  </si>
+  <si>
+    <t>What is the name of the distribution site?</t>
+  </si>
+  <si>
+    <t>thanks</t>
+  </si>
+  <si>
+    <t>Thank you for completing the post-distribution survey. Continue to the next screen to finalize.</t>
+  </si>
+  <si>
+    <t>Would you like to scan a different item pack instead?</t>
+  </si>
+  <si>
+    <t>no_report_option</t>
+  </si>
+  <si>
+    <t>Since no item pack was successfully distributed, we will not fill out a post-distribution report.</t>
+  </si>
+  <si>
+    <t>clause</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>values_list</t>
+  </si>
+  <si>
+    <t>display.hint</t>
+  </si>
+  <si>
+    <t>branch_label</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>model.isSessionVariable</t>
+  </si>
+  <si>
+    <t>distribution</t>
+  </si>
+  <si>
+    <t>query_name</t>
+  </si>
+  <si>
+    <t>query_type</t>
+  </si>
+  <si>
+    <t>linked_form_id</t>
+  </si>
+  <si>
+    <t>linked_table_id</t>
+  </si>
+  <si>
+    <t>selection</t>
+  </si>
+  <si>
+    <t>selectionArgs</t>
+  </si>
+  <si>
+    <t>fieldName</t>
+  </si>
+  <si>
+    <t>auxillaryHash</t>
+  </si>
+  <si>
+    <t>prompt_type_name</t>
+  </si>
+  <si>
+    <t>Deployment To Specific</t>
+  </si>
+  <si>
     <t>number</t>
   </si>
   <si>
-    <t>min_range</t>
-  </si>
-  <si>
-    <t>max_range</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>pre-deployment</t>
-  </si>
-  <si>
-    <t>We will now distribute the appropriate item pack</t>
-  </si>
-  <si>
-    <t>barcode</t>
-  </si>
-  <si>
-    <t>Scan an item pack barcode within the range of {{data.min_range}} to {{data.max_range}}</t>
-  </si>
-  <si>
-    <t>item_scan</t>
-  </si>
-  <si>
-    <t>if</t>
-  </si>
-  <si>
-    <t>(data('scanned_item_pack_barcode') &gt; data('maxRange')) || (data('scanned_item_pack_barcode') &lt; data('minRange'))</t>
-  </si>
-  <si>
-    <t>select_one</t>
-  </si>
-  <si>
-    <t>try_again</t>
-  </si>
-  <si>
-    <t>Unauthorized Item Pack! Do not distribute this  item pack. Would you like to scan a different item pack?</t>
-  </si>
-  <si>
-    <t>selected(data('try_again'),'yes')</t>
-  </si>
-  <si>
-    <t>goto item_scan</t>
-  </si>
-  <si>
-    <t>end if</t>
-  </si>
-  <si>
-    <t>else</t>
-  </si>
-  <si>
-    <t>This item pack is authorized. Please distribute this item pack.</t>
-  </si>
-  <si>
-    <t>linked_table</t>
-  </si>
-  <si>
-    <t>Please click the pencil icon to record distribution</t>
-  </si>
-  <si>
-    <t>begin screen</t>
-  </si>
-  <si>
-    <t>Please continue to the next screen if you have clicked the pencil icon to record distribution</t>
-  </si>
-  <si>
-    <t>async_assign_single_string</t>
-  </si>
-  <si>
-    <t>is_distributed_value_query</t>
-  </si>
-  <si>
-    <t>end screen</t>
-  </si>
-  <si>
-    <t>data('is_distributed') == 'true'</t>
-  </si>
-  <si>
-    <t>pre-summary</t>
-  </si>
-  <si>
-    <t>Since the authorized item pack was successfully distributed, we will complete now complete a brief report.</t>
-  </si>
-  <si>
-    <t>assign</t>
-  </si>
-  <si>
-    <t>now()</t>
-  </si>
-  <si>
-    <t>What is the name of the distributor?</t>
-  </si>
-  <si>
-    <t>What is the name of the distribution site?</t>
-  </si>
-  <si>
-    <t>thanks</t>
-  </si>
-  <si>
-    <t>Thank you for completing the post-distribution survey. Continue to the next screen to finalize.</t>
-  </si>
-  <si>
-    <t>Would you like to scan a different item pack instead?</t>
-  </si>
-  <si>
-    <t>no_report_option</t>
-  </si>
-  <si>
-    <t>Since no item pack was successfully distributed, we will not fill out a post-distribution report.</t>
-  </si>
-  <si>
-    <t>clause</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>values_list</t>
-  </si>
-  <si>
-    <t>display.hint</t>
-  </si>
-  <si>
-    <t>branch_label</t>
-  </si>
-  <si>
-    <t>calculation</t>
-  </si>
-  <si>
-    <t>model.isSessionVariable</t>
-  </si>
-  <si>
-    <t>distribution</t>
-  </si>
-  <si>
-    <t>query_name</t>
-  </si>
-  <si>
-    <t>query_type</t>
-  </si>
-  <si>
-    <t>linked_form_id</t>
-  </si>
-  <si>
-    <t>linked_table_id</t>
-  </si>
-  <si>
-    <t>selection</t>
-  </si>
-  <si>
-    <t>selectionArgs</t>
-  </si>
-  <si>
-    <t>fieldName</t>
-  </si>
-  <si>
-    <t>auxillaryHash</t>
-  </si>
-  <si>
-    <t>prompt_type_name</t>
-  </si>
-  <si>
-    <t>Deployment To Specific</t>
-  </si>
-  <si>
-    <t>[data('distribution_id')]</t>
-  </si>
-  <si>
-    <t>'distribution_id='+opendatakit.encodeURIDataElement('distribution_id')</t>
-  </si>
-  <si>
-    <t>distribution _id = ?</t>
+    <t>[data('beneficiary_code'), data('distribution_id')]</t>
+  </si>
+  <si>
+    <t>'beneficiary_code='+opendatakit.encodeURIDataElement('beneficiary_code')+ '&amp;_id='+opendatakit.encodeURIDataElement('distribution_id')</t>
+  </si>
+  <si>
+    <t>beneficiary_code = ? and distribution_id = ?</t>
+  </si>
+  <si>
+    <t>set_is_distributed</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -543,7 +546,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,7 +880,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -993,18 +995,18 @@
     </row>
     <row r="14" spans="1:2" ht="23">
       <c r="A14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="23">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1076,7 +1078,7 @@
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="23">
@@ -1177,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1196,16 +1198,16 @@
   <sheetData>
     <row r="1" spans="1:21" ht="23">
       <c r="A1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" s="31" t="s">
         <v>1</v>
@@ -1214,30 +1216,30 @@
         <v>30</v>
       </c>
       <c r="G1" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" t="s">
         <v>81</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>82</v>
-      </c>
-      <c r="J1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="23">
       <c r="A2" s="12"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="19"/>
@@ -1259,18 +1261,18 @@
       <c r="A3" s="20"/>
       <c r="B3" s="21"/>
       <c r="C3" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="25"/>
       <c r="H3" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -1288,10 +1290,10 @@
     </row>
     <row r="4" spans="1:21" ht="23">
       <c r="A4" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>49</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -1317,16 +1319,16 @@
       <c r="A5" s="20"/>
       <c r="B5" s="21"/>
       <c r="C5" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>51</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>52</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="26"/>
@@ -1348,10 +1350,10 @@
     </row>
     <row r="6" spans="1:21" ht="23">
       <c r="A6" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -1375,7 +1377,7 @@
     </row>
     <row r="7" spans="1:21" ht="23">
       <c r="A7" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="22"/>
@@ -1400,7 +1402,7 @@
     </row>
     <row r="8" spans="1:21" ht="23">
       <c r="A8" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
@@ -1425,7 +1427,7 @@
     </row>
     <row r="9" spans="1:21" ht="23">
       <c r="A9" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>
@@ -1452,12 +1454,12 @@
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
       <c r="C10" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
       <c r="F10" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
@@ -1479,14 +1481,14 @@
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
       <c r="C11" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="26"/>
@@ -1506,7 +1508,7 @@
     </row>
     <row r="12" spans="1:21" ht="23">
       <c r="A12" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
@@ -1531,7 +1533,7 @@
     </row>
     <row r="13" spans="1:21" ht="23">
       <c r="A13" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -1558,12 +1560,12 @@
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
       <c r="F14" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="26"/>
@@ -1585,10 +1587,10 @@
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>63</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>8</v>
@@ -1635,7 +1637,7 @@
     </row>
     <row r="17" spans="1:21" ht="23">
       <c r="A17" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="22"/>
@@ -1660,10 +1662,10 @@
     </row>
     <row r="18" spans="1:21" ht="23">
       <c r="A18" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
@@ -1689,14 +1691,14 @@
       <c r="A19" s="20"/>
       <c r="B19" s="21"/>
       <c r="C19" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>67</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="26"/>
@@ -1718,7 +1720,7 @@
       <c r="A20" s="20"/>
       <c r="B20" s="21"/>
       <c r="C20" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="23" t="s">
@@ -1728,7 +1730,7 @@
       <c r="G20" s="25"/>
       <c r="H20" s="26"/>
       <c r="I20" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
@@ -1754,7 +1756,7 @@
         <v>7</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
@@ -1783,7 +1785,7 @@
         <v>6</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="25"/>
       <c r="H22" s="26"/>
@@ -1805,14 +1807,14 @@
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="24" t="s">
         <v>72</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>73</v>
       </c>
       <c r="G23" s="25"/>
       <c r="H23" s="26"/>
@@ -1832,7 +1834,7 @@
     </row>
     <row r="24" spans="1:21" ht="23">
       <c r="A24" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
@@ -1859,16 +1861,16 @@
       <c r="A25" s="20"/>
       <c r="B25" s="21"/>
       <c r="C25" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
@@ -1888,10 +1890,10 @@
     </row>
     <row r="26" spans="1:21" ht="23">
       <c r="A26" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
@@ -1915,7 +1917,7 @@
     </row>
     <row r="27" spans="1:21" ht="23">
       <c r="A27" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
@@ -1940,7 +1942,7 @@
     </row>
     <row r="28" spans="1:21" ht="23">
       <c r="A28" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
@@ -1967,14 +1969,14 @@
       <c r="A29" s="20"/>
       <c r="B29" s="21"/>
       <c r="C29" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="24" t="s">
         <v>75</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>76</v>
       </c>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
@@ -1996,7 +1998,7 @@
     </row>
     <row r="30" spans="1:21" ht="23">
       <c r="A30" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
@@ -2021,7 +2023,7 @@
     </row>
     <row r="31" spans="1:21" ht="23">
       <c r="A31" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
@@ -2056,68 +2058,67 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>90</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>91</v>
       </c>
-      <c r="H1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="17" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="18" customHeight="1">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="4" spans="1:9">
+    </row>
+    <row r="4" spans="1:8">
       <c r="H4" s="11"/>
     </row>
   </sheetData>
@@ -2142,7 +2143,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="30">
       <c r="A1" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>0</v>
@@ -2150,7 +2151,7 @@
     </row>
     <row r="2" spans="1:2" ht="45">
       <c r="A2" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>2</v>

</xml_diff>